<commit_message>
Added a couple of changes to committee page, added descriptions for committees to spreadsheet
</commit_message>
<xml_diff>
--- a/idb_project_data.xlsx
+++ b/idb_project_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="5190"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="5190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="374">
   <si>
     <t>Description</t>
   </si>
@@ -518,13 +519,7 @@
     <t>Businessman, investor</t>
   </si>
   <si>
-    <t>This committee handles the flow of legislation in a number of policy areas, including water resources, air quality, oil and gas, waste, and parks and wildlife.</t>
-  </si>
-  <si>
     <t>Natural Resources</t>
-  </si>
-  <si>
-    <t>This committee addresses crucial statewide issues impacting all Texans.</t>
   </si>
   <si>
     <t xml:space="preserve"> Senate Member, 2013 – present</t>
@@ -1308,12 +1303,60 @@
   <si>
     <t>http://www.legis.state.tx.us/BillLookup/BillStages.aspx?LegSess=83R&amp;Bill=SB748</t>
   </si>
+  <si>
+    <t xml:space="preserve">Develop and implement cost efficiences in structure andDevelop and implement cost efficiencies in structure and operation of the Texas Senate, review legislative resources available to the Legislature and the public, and make recommendations to enhance availability and transparency of governmental information. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review cases involving the imposition of probation rather than imprisonment or commitment for adult and juvenile intoxication manslaughter offenders and ensure that sentences include appropriate punishment levels, maintain public safety, and serve to deter driving under the influence. Also, study the operations of Texas prison system with respect to the medical and mental health care treatment.  Furthermore, study and make recommendations related to jail diversion, reduced recidivism rates, and access to services for those within the system who suffer from a mental illness. </t>
+  </si>
+  <si>
+    <t>Study current legislative and regulatory barriers that could impede capital investment, growth, and expansion of Texas businesses, Project and examine the costs and economic impact to Texas businesses in complying with the federal health care law, study and make recommendations to develop a biennial state review process for economic development programs to determine their effectiveness in keeping Texas economically competitive while ensuring taxpayer dollars are used wisely, and monitor implementation of SB 21 (83-R), which requires drug testing for unemployment insurance claimants.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examine the current regulatory and insurance requirements for the storage of ammonium nitrate, including the role of the State Chemist and the Texas Department of Insurance, examine the role of state and local governments regarding recovery operations across the state in the event of a disaster, monitor the state's efforts to secure the border, including the state's increased investment in border security during the 83rd legislative session, study the current practice of reporting crime statistics in Texas, including border security crime statistics, and tudy and make recommendations on removing barriers to Second Amendment Rights, including but not limited to open carry Examine the current regulatory and insurance requirements for the storage of ammonium nitrate, including the role of the State Chemist and the Texas Department of Insurance, examine the role of state and local governments regarding recovery operations across the state in the event of a disaster, monitor the state's efforts to secure the border, including the state's increased investment in border security during the 83rd legislative session, study the current practice of reporting crime statistics in Texas, including border security crime statistics, and study and make recommendations on removing barriers to Second Amendment Rights, including but not limited to open carry legislation.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examine STAAR writing scores for elementary, middle and high school students and monitor the implementation of legislation addressed by the Senate Committee on Education, 83rd Legislature, Regular and Called Sessions, and make recommendations for any legislation needed to improve, enhance and/or complete implementation. </t>
+  </si>
+  <si>
+    <t>Examine state agencies' mandated reporting practices, the necessity and utility of these reports, and reporting processes to the legislature and to the public, review and recommend improvements to state agency training, policies, and procedures for monitoring and reporting performance of state contracts, including a review of exemptions to state contracting oversight, and monitor the implementation of SB 1597, relating to the development of state agency information security plans to improve the security of agency information systems and to proactively protect the state against cybercrime and similar security threats.</t>
+  </si>
+  <si>
+    <t>Review and evaluate the success of Closing the Gaps by 2015, the strategic plan for higher education adopted in 2000, study and make recommendations regarding the impact of technology on higher education instruction, including online courses and massive open online courses (MOOCs), and their impact on higher education excellence, cost, and funding requirements, and monitor the implementation of legislation addressed by the Senate Committee on Higher Education, 83rd Legislature, Regular and Called Sessions, and make recommendations for any legislation needed to improve, enhance and/or complete implementation.</t>
+  </si>
+  <si>
+    <t>Review the Department of Family and Protective Services' efforts to reduce child fatalities, monitor the implementation of programs that were created or expanded by the 83rd Legislature to improve mental health and substance abuse services and assess these efforts' contribution to improved outcomes such as reduced recidivism in state hospitals, diversion from emergency rooms and county jails, and access to permanent supportive housing. Identify and address gaps in the current mental health and substance abuse system and make recommendations to better coordinate services across agencies and programs, build on previous legislative achievements in women's healthcare by examining women's access to preventative health care, pregnancy services, and post-partum care, and exploring ways to expand access and improve quality, particularly in rural and underserved areas of the state, identify cost-effective alternatives to Medicaid and the Affordable Care Act to better connect low income individuals to health care services through private market-based solutions, including Medicaid block grants and waivers, valuate the Temporary Assistance for Needy Families (TANF) program structure. Make recommendations to improve the program's operations and ensure the program achieves outcomes that allow TANF recipients to find employment and achieve self-sufficiency, evaluate the current state of prescription drug abuse and strategies for reducing prescription drug abuse in Texas and monitor the implementation of legislation addressed by the Senate Committee on Health and Human Services, 83rd Legislature, Regular Session, and make recommendations for any legislation needed to improve, enhance, and/or complete implementation.</t>
+  </si>
+  <si>
+    <t>Study and make recommendations to increase transparency in the authorization, issuance, and appropriation of debt at the local level and examine the immediate and long-term fiscal impact that bonds and other types of obligations issued by local governments have on current and future generations of taxpayers.</t>
+  </si>
+  <si>
+    <t>Monitor the implementation of Senate Bill 393 and Senate Bill 1114 and determine if any statutory changes are necessary to clarify the intent of this legislation. In addition, determine those school districts that have implemented the graduated sanctions envisioned by Senate Bill 393 and decide if any additional statutory changes are necessary to ensure that school districts are complying with its intent. Also, monitor the implementation of statewide electronic filing as mandated by the Texas Supreme Court to determine if any additional training or resources are needed by local jurisdictions.</t>
+  </si>
+  <si>
+    <t>Study and make recommendations to encourage the use of brackish water including but not limited to Aquifer Storage and Recovery and Desalination, study and make recommendations on what state and federal environmental regulations most affect implementation of water supply strategies in the State Water Plan, including recommendations to reduce state barriers, examine current processes for environmental permitting, including the impact of permitting delays on economic development, and monitor implementation of legislation passed during the 83rd Legislative Session including monitoring implementation of House Bill 4, creating the state water implementation fund.</t>
+  </si>
+  <si>
+    <t>Review the Texas Public Information Act to ensure that access to public records and information by the public remains fully transparent, but that governmental entities have the authority to protect the privacy interests of citizens, including primary and higher education students, from improper public disclosure and review and make recommendations on improving the transparency of information available on state websites regarding state expenditures, reports, and contracts, including a comparison of how similar information is provided by other states.</t>
+  </si>
+  <si>
+    <t>Examine the anticipated impact increased oil and gas production will continue to have on roadways and bridges, evaluate the Texas Department of Transportation and Metropolitan Planning Organization's progress on reducing congestion on the 100 Most Congested Roadway segments and make recommendations to advance the development of the remaining congestion relief projects, evaluate Comprehensive Development Agreements (CDA) and Design/Build project delivery methods and make recommendations for their future role in reducing congestion and continuing the state's economic growth, and examine the implementation of SB 1792 (83R), which provides remedies for habitual violators of nonpayment of tolls and make recommendations for any legislation needed to improve, enhance, and/or complete implementation.</t>
+  </si>
+  <si>
+    <t>Investigate the impact of federal actions (including the federal government shutdown, sequestration, military force reductions, and potential base closure or realignment) on active-duty service members, the Texas Military Department, veterans, their families, defense-related contractors, small businesses, local governments, and state agencies, monitor and examine efforts to provide employment and workforce opportunities for veterans, service members, and their families, provide an update on the State Strike Force teams' progress and recommendations on any additional steps necessary to ensure that veterans promptly receive all federal disability benefits to which they are entitled, and study and make recommendations to improve access to services provided by non-profit organizations to veterans, their families, and survivors, including examining the effectiveness, standards, and consistency of the 2-1-1 information and referral system for military and veteran families statewide.</t>
+  </si>
+  <si>
+    <t>Examine the negative economic impact on Texas business from legal issues involving threatened and actual patent litigation by "patent assertion entities" (PAEs) impacting all Texans, examine possible measures to protect the personal privacy of Texas residents from governmental and commercial surveillance, review the types and scope of personal data collected by governmental and commercial entities and consider methods to minimize the government's collection of data on its citizens, examine possible reforms designed to increase citizens' ability to know what data is being collected about them by governmental and commercial entities and with whom that data is being shared, study the online legislative resources available to the public from Texas Senate Committee websites and compare resources to those provided by other state legislative committees in Texas and other states, study the emerging negative impacts of the Federal Affordable Care Act, and study and make recommendations on increasing medical price transparency in Texas, including studying the impact of SB 1731, 80th Legislative Session.</t>
+  </si>
+  <si>
+    <t>Review the administrative and financial state of the Texas Windstorm Insurance Association (TWIA), review the Texas FAIR Plan's organizational and financial structure as the state's insurer of last resort for residential homeowner's insurance coverage, and monitor the implementation of advanced metering infrastructure to ensure minimization of utility customer costs.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1414,6 +1457,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000033"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1507,7 +1556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1664,6 +1713,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1970,7 +2022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2210,16 +2262,16 @@
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>340</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>341</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>342</v>
-      </c>
       <c r="D8" s="25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>11</v>
@@ -2237,21 +2289,21 @@
         <v>12</v>
       </c>
       <c r="J8" s="54" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C9" s="55" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E9" s="55" t="s">
         <v>11</v>
@@ -2269,21 +2321,21 @@
         <v>12</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C10" s="55" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="55" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E10" s="55" t="s">
         <v>11</v>
@@ -2301,18 +2353,18 @@
         <v>12</v>
       </c>
       <c r="J10" s="54" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>348</v>
+      </c>
+      <c r="C11" s="55" t="s">
         <v>349</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>350</v>
-      </c>
-      <c r="C11" s="55" t="s">
-        <v>351</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>16</v>
@@ -2333,18 +2385,18 @@
         <v>12</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="91.5" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="C12" s="55" t="s">
         <v>353</v>
-      </c>
-      <c r="B12" s="55" t="s">
-        <v>354</v>
-      </c>
-      <c r="C12" s="55" t="s">
-        <v>355</v>
       </c>
       <c r="D12" s="55" t="s">
         <v>16</v>
@@ -2365,21 +2417,21 @@
         <v>12</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="91.5" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C13" s="55" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>11</v>
@@ -2397,7 +2449,7 @@
         <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -2495,7 +2547,7 @@
         <v>90</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>8</v>
@@ -2531,7 +2583,7 @@
         <v>91</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>37</v>
@@ -2565,7 +2617,7 @@
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>39</v>
@@ -2578,10 +2630,10 @@
         <v>83</v>
       </c>
       <c r="L4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
@@ -2637,7 +2689,7 @@
         <v>96</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="2"/>
@@ -2671,18 +2723,18 @@
         <v>102</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H7" s="31"/>
       <c r="I7" s="33"/>
       <c r="J7" s="33" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K7" s="33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="99" customHeight="1" x14ac:dyDescent="0.25">
@@ -2705,7 +2757,7 @@
         <v>107</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2739,7 +2791,7 @@
         <v>116</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="2"/>
@@ -2773,7 +2825,7 @@
         <v>122</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="2"/>
@@ -2807,15 +2859,15 @@
         <v>127</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L11" t="s">
         <v>128</v>
@@ -2841,15 +2893,15 @@
         <v>91</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L12" t="s">
         <v>132</v>
@@ -2866,7 +2918,7 @@
         <v>135</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
@@ -2875,7 +2927,7 @@
         <v>134</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="2"/>
@@ -2905,18 +2957,18 @@
         <v>138</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2930,7 +2982,7 @@
         <v>156</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E15" s="6">
         <v>24</v>
@@ -2939,14 +2991,14 @@
         <v>155</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2960,27 +3012,27 @@
         <v>32</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E16" s="6">
         <v>6</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2991,30 +3043,30 @@
         <v>28</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E17" s="31">
         <v>9</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3025,33 +3077,33 @@
         <v>28</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E18" s="42">
         <v>18</v>
       </c>
       <c r="F18" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3065,30 +3117,30 @@
         <v>32</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E19" s="50">
         <v>20</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3099,33 +3151,33 @@
         <v>44</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E20" s="6">
         <v>27</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L20" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3136,31 +3188,31 @@
         <v>28</v>
       </c>
       <c r="C21" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="E21" s="6">
         <v>3</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3171,10 +3223,10 @@
         <v>28</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E22" s="6">
         <v>7</v>
@@ -3183,21 +3235,21 @@
         <v>91</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -3208,38 +3260,38 @@
         <v>28</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E23" s="6">
         <v>8</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>44</v>
@@ -3248,30 +3300,30 @@
         <v>32</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E24" s="6">
         <v>29</v>
       </c>
       <c r="F24" s="40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="93" customHeight="1" x14ac:dyDescent="0.25">
@@ -3282,33 +3334,33 @@
         <v>28</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E25" s="6">
         <v>5</v>
       </c>
       <c r="F25" s="40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M25" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3319,33 +3371,33 @@
         <v>28</v>
       </c>
       <c r="C26" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>229</v>
       </c>
       <c r="E26" s="6">
         <v>31</v>
       </c>
       <c r="F26" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="G26" s="30" t="s">
         <v>228</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>230</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L26" s="25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
@@ -3356,33 +3408,33 @@
         <v>28</v>
       </c>
       <c r="C27" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="E27" s="6">
         <v>11</v>
       </c>
       <c r="F27" s="40" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K27" s="41" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3393,10 +3445,10 @@
         <v>44</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E28" s="6">
         <v>19</v>
@@ -3405,21 +3457,21 @@
         <v>103</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K28" s="41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3433,30 +3485,30 @@
         <v>32</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E29" s="6">
         <v>14</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K29" s="41" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M29" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3467,10 +3519,10 @@
         <v>44</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E30" s="6">
         <v>23</v>
@@ -3479,21 +3531,21 @@
         <v>107</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K30" s="41" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L30" s="25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3507,7 +3559,7 @@
         <v>32</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E31" s="6">
         <v>15</v>
@@ -3516,21 +3568,21 @@
         <v>91</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K31" s="41" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L31" s="25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -3590,8 +3642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,7 +3680,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>65</v>
       </c>
@@ -3638,7 +3690,9 @@
       <c r="C2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="D2" s="18" t="s">
+        <v>365</v>
+      </c>
       <c r="E2" s="19" t="s">
         <v>70</v>
       </c>
@@ -3649,7 +3703,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -3659,7 +3713,9 @@
       <c r="C3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="18"/>
+      <c r="D3" s="18" t="s">
+        <v>359</v>
+      </c>
       <c r="E3" s="20">
         <v>41282</v>
       </c>
@@ -3670,7 +3726,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>47</v>
       </c>
@@ -3681,7 +3737,7 @@
         <v>67</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>159</v>
+        <v>372</v>
       </c>
       <c r="E4" s="20">
         <v>41282</v>
@@ -3693,9 +3749,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>133</v>
@@ -3703,16 +3759,18 @@
       <c r="C5" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="45" t="s">
+        <v>358</v>
+      </c>
       <c r="E5" s="45"/>
       <c r="F5" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>137</v>
@@ -3720,16 +3778,18 @@
       <c r="C6" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="45" t="s">
+        <v>361</v>
+      </c>
       <c r="E6" s="45"/>
       <c r="F6" s="47" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G6" s="18"/>
     </row>
-    <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B7" s="45" t="s">
         <v>106</v>
@@ -3737,16 +3797,18 @@
       <c r="C7" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="45"/>
+      <c r="D7" s="45" t="s">
+        <v>373</v>
+      </c>
       <c r="E7" s="45"/>
       <c r="F7" s="47" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B8" s="45" t="s">
         <v>67</v>
@@ -3754,50 +3816,54 @@
       <c r="C8" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="D8" s="45"/>
+      <c r="D8" s="45" t="s">
+        <v>360</v>
+      </c>
       <c r="E8" s="45"/>
       <c r="F8" s="47" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B9" s="46" t="s">
         <v>147</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>300</v>
-      </c>
-      <c r="D9" s="45"/>
+        <v>298</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>362</v>
+      </c>
       <c r="E9" s="45"/>
       <c r="F9" s="45" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="46" t="s">
         <v>302</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>303</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>304</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="45"/>
       <c r="F10" s="45" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B11" s="45" t="s">
         <v>42</v>
@@ -3805,67 +3871,75 @@
       <c r="C11" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="45"/>
+      <c r="D11" s="45" t="s">
+        <v>363</v>
+      </c>
       <c r="E11" s="45"/>
       <c r="F11" s="45" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B12" s="46" t="s">
         <v>150</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>308</v>
-      </c>
-      <c r="D12" s="45"/>
+        <v>306</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>364</v>
+      </c>
       <c r="E12" s="45"/>
       <c r="F12" s="45" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="315" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>310</v>
-      </c>
-      <c r="D13" s="45"/>
+        <v>308</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>366</v>
+      </c>
       <c r="E13" s="45"/>
       <c r="F13" s="45" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B14" s="45" t="s">
         <v>154</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="D14" s="45"/>
+        <v>273</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>367</v>
+      </c>
       <c r="E14" s="45"/>
       <c r="F14" s="45" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15" s="45" t="s">
         <v>140</v>
@@ -3874,17 +3948,17 @@
         <v>137</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>157</v>
+        <v>368</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="45" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B16" s="45" t="s">
         <v>143</v>
@@ -3895,30 +3969,32 @@
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
       <c r="F16" s="45" t="s">
+        <v>313</v>
+      </c>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" s="45" t="s">
         <v>315</v>
-      </c>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
-        <v>316</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>317</v>
       </c>
       <c r="C17" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="45"/>
+      <c r="D17" s="58" t="s">
+        <v>369</v>
+      </c>
       <c r="E17" s="45"/>
       <c r="F17" s="45" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>146</v>
@@ -3926,16 +4002,18 @@
       <c r="C18" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="45"/>
+      <c r="D18" s="45" t="s">
+        <v>370</v>
+      </c>
       <c r="E18" s="45"/>
       <c r="F18" s="45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B19" s="45" t="s">
         <v>50</v>
@@ -3943,10 +4021,12 @@
       <c r="C19" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="45"/>
+      <c r="D19" s="45" t="s">
+        <v>371</v>
+      </c>
       <c r="E19" s="45"/>
       <c r="F19" s="45" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -3958,5 +4038,6 @@
     <hyperlink ref="B12" r:id="rId5" display="http://www.seliger.senate.state.tx.us/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>